<commit_message>
add valdiation check before vlan creation - cisco & junos
</commit_message>
<xml_diff>
--- a/network_devices.xlsx
+++ b/network_devices.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\library\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD1F232-3E5D-4C3C-8699-A6BA1EE0B5F3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDBC33F-D3FD-4ABE-90C1-C4EDCA6413E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="2805" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -711,7 +711,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,7 +753,7 @@
         <v>19</v>
       </c>
       <c r="E2" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -829,7 +829,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>5</v>
@@ -838,7 +838,7 @@
         <v>20</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -846,7 +846,7 @@
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>6</v>

</xml_diff>

<commit_message>
Add group called test_junos for testing purposes
</commit_message>
<xml_diff>
--- a/network_devices.xlsx
+++ b/network_devices.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\infra_new_vlan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="R:\infra_new_vlan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DDBC33F-D3FD-4ABE-90C1-C4EDCA6413E7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -18,11 +17,11 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$14</definedName>
-    <definedName name="groups">'Data types'!$E$6:$E$8</definedName>
+    <definedName name="groups">'Data types'!$E$6:$E$9</definedName>
     <definedName name="models">'Data types'!$F$6:$F$9</definedName>
     <definedName name="types">'Data types'!$G$6:$G$7</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -35,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="34">
   <si>
     <t>Caption</t>
   </si>
@@ -128,12 +127,21 @@
   </si>
   <si>
     <t>PTSWCORE1</t>
+  </si>
+  <si>
+    <t>192.168.20.244</t>
+  </si>
+  <si>
+    <t>home-qfx</t>
+  </si>
+  <si>
+    <t>test_junos</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -460,23 +468,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -512,23 +503,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -704,25 +678,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
         <v>4</v>
       </c>
@@ -739,12 +713,12 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="s">
         <v>9</v>
       </c>
       <c r="B2" s="14" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C2" s="14" t="s">
         <v>12</v>
@@ -756,7 +730,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="13" t="s">
         <v>7</v>
       </c>
@@ -773,7 +747,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
@@ -790,7 +764,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="13" t="s">
         <v>10</v>
       </c>
@@ -807,7 +781,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="13" t="s">
         <v>11</v>
       </c>
@@ -824,12 +798,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="13" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>16</v>
+        <v>26</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>5</v>
@@ -841,12 +815,12 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>1</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>6</v>
@@ -858,7 +832,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="13" t="s">
         <v>29</v>
       </c>
@@ -875,119 +849,129 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13"/>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="15"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A10" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E10" s="15" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="13"/>
       <c r="B11" s="14"/>
       <c r="C11" s="14"/>
       <c r="D11" s="14"/>
       <c r="E11" s="15"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="13"/>
       <c r="B12" s="14"/>
       <c r="C12" s="14"/>
       <c r="D12" s="14"/>
       <c r="E12" s="15"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="13"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
       <c r="D13" s="14"/>
       <c r="E13" s="15"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="13"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
       <c r="D14" s="14"/>
       <c r="E14" s="15"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="13"/>
       <c r="B15" s="14"/>
       <c r="C15" s="14"/>
       <c r="D15" s="14"/>
       <c r="E15" s="15"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="13"/>
       <c r="B16" s="14"/>
       <c r="C16" s="14"/>
       <c r="D16" s="14"/>
       <c r="E16" s="15"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="13"/>
       <c r="B17" s="14"/>
       <c r="C17" s="14"/>
       <c r="D17" s="14"/>
       <c r="E17" s="15"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="13"/>
       <c r="B18" s="14"/>
       <c r="C18" s="14"/>
       <c r="D18" s="14"/>
       <c r="E18" s="15"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="13"/>
       <c r="B19" s="14"/>
       <c r="C19" s="14"/>
       <c r="D19" s="14"/>
       <c r="E19" s="15"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
       <c r="D20" s="14"/>
       <c r="E20" s="15"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="13"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
       <c r="D21" s="14"/>
       <c r="E21" s="15"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
       <c r="D22" s="14"/>
       <c r="E22" s="15"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="13"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
       <c r="D23" s="14"/>
       <c r="E23" s="15"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="13"/>
       <c r="B24" s="14"/>
       <c r="C24" s="14"/>
       <c r="D24" s="14"/>
       <c r="E24" s="15"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="13"/>
       <c r="B25" s="14"/>
       <c r="C25" s="14"/>
       <c r="D25" s="14"/>
       <c r="E25" s="15"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A26" s="16"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
@@ -995,16 +979,16 @@
       <c r="E26" s="18"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E14" xr:uid="{F64965F6-A56A-4704-8363-1DA37AA83CC2}"/>
+  <autoFilter ref="A1:E14"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26" xr:uid="{9CF9407C-3E0F-40A2-96BE-F46D73BC4CE6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B26">
       <formula1>groups</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D26" xr:uid="{D5B28DCE-D7C8-40FE-AFE8-5799DA5100F6}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D2:D26">
       <formula1>models</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E26" xr:uid="{28426E06-D5D7-4966-84F0-0103B171A9C2}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E2:E26">
       <formula1>types</formula1>
     </dataValidation>
   </dataValidations>
@@ -1015,24 +999,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="E4:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="5" max="5" width="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E5" s="2" t="s">
         <v>28</v>
       </c>
@@ -1043,7 +1027,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
@@ -1054,7 +1038,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E7" s="5" t="s">
         <v>27</v>
       </c>
@@ -1065,58 +1049,60 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E8" s="5" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="F8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="G8" s="6"/>
     </row>
-    <row r="9" spans="5:7" x14ac:dyDescent="0.25">
-      <c r="E9" s="5"/>
+    <row r="9" spans="5:7" x14ac:dyDescent="0.3">
+      <c r="E9" s="5" t="s">
+        <v>26</v>
+      </c>
       <c r="F9" s="1" t="s">
         <v>24</v>
       </c>
       <c r="G9" s="6"/>
     </row>
-    <row r="10" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E10" s="5"/>
       <c r="F10" s="1"/>
       <c r="G10" s="6"/>
     </row>
-    <row r="11" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E11" s="5"/>
       <c r="F11" s="1"/>
       <c r="G11" s="6"/>
     </row>
-    <row r="12" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E12" s="5"/>
       <c r="F12" s="1"/>
       <c r="G12" s="6"/>
     </row>
-    <row r="13" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E13" s="5"/>
       <c r="F13" s="1"/>
       <c r="G13" s="6"/>
     </row>
-    <row r="14" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E14" s="5"/>
       <c r="F14" s="1"/>
       <c r="G14" s="6"/>
     </row>
-    <row r="15" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E15" s="5"/>
       <c r="F15" s="1"/>
       <c r="G15" s="6"/>
     </row>
-    <row r="16" spans="5:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="5:7" x14ac:dyDescent="0.3">
       <c r="E16" s="5"/>
       <c r="F16" s="1"/>
       <c r="G16" s="6"/>
     </row>
-    <row r="17" spans="5:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="E17" s="7"/>
       <c r="F17" s="8"/>
       <c r="G17" s="9"/>

</xml_diff>